<commit_message>
Cập nhật Automation Test cho chức năng quản lý sản phẩm và thêm file excel có sửa pom
</commit_message>
<xml_diff>
--- a/src/test/resources/TestLoginData.xlsx
+++ b/src/test/resources/TestLoginData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="53">
   <si>
     <t>STT</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>Security Active: Redirected to http://localhost:8080/auth/login?error=Access-Denied-Admin-Only</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/home/index;jsessionid=FF060E78F79C609A0474E1C28AD3349E</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/home/index;jsessionid=5B0E62695885E2E489F4764B6A4AD689</t>
   </si>
 </sst>
 </file>
@@ -635,7 +641,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>29</v>
@@ -658,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>29</v>

</xml_diff>

<commit_message>
Tích hợp thanh toán VNPay = Demo Sandbox VNPayment SDK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestLoginData.xlsx
+++ b/src/test/resources/TestLoginData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="57">
   <si>
     <t>STT</t>
   </si>
@@ -203,6 +203,27 @@
   </si>
   <si>
     <t>http://localhost:8080/home/index;jsessionid=5B0E62695885E2E489F4764B6A4AD689</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/home/index;jsessionid=3739F55CD6E94CEB4939ECE611151955</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/home/index;jsessionid=6B0318CE559D0A7BC7BE5786AE212B2F</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/home/index;jsessionid=647D78420C01EDFF052B79870B73076D</t>
+  </si>
+  <si>
+    <t>Lỗi: no such window: target window already closed
+from unknown error: web view not found
+  (Session info: chrome=145.0.7632.76)
+Build info: version: '4.14.1', revision: '03f8ede370'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [b5d05d6c08870a977d15179599401354, sendKeysToElement {id=f.F24A41F9119A8E04E81E2562BC6393EE.d.48E05C2B15138ED5E3632BC7F8322B81.e.4, value=[Ljava.lang.CharSequence;@68868328}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.76, chrome: {chromedriverVersion: 145.0.7632.77 (da516187054a..., userDataDir: C:\Users\DELL\AppData\Local...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50697}, goog:processID: 1616, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50697/devtoo..., se:cdpVersion: 145.0.7632.76, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Element: [[ChromeDriver: chrome on windows (b5d05d6c08870a977d15179599401354)] -&gt; name: password]
+Session ID: b5d05d6c08870a977d15179599401354</t>
   </si>
 </sst>
 </file>
@@ -641,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>29</v>
@@ -664,10 +685,10 @@
         <v>5</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>

</xml_diff>